<commit_message>
Set 0 initial value for stepPosition
</commit_message>
<xml_diff>
--- a/src/tests/AngleTest/AngleTest.xlsx
+++ b/src/tests/AngleTest/AngleTest.xlsx
@@ -26,19 +26,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">Input in Deg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umdrehungen (Stange)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -125,7 +129,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -140,6 +144,10 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -214,7 +222,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -618,11 +626,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="96572251"/>
-        <c:axId val="70600091"/>
+        <c:axId val="54465415"/>
+        <c:axId val="25729537"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96572251"/>
+        <c:axId val="54465415"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,12 +662,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70600091"/>
+        <c:crossAx val="25729537"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70600091"/>
+        <c:axId val="25729537"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -698,7 +706,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96572251"/>
+        <c:crossAx val="54465415"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -726,7 +734,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1122,11 +1130,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="27635355"/>
-        <c:axId val="54158381"/>
+        <c:axId val="94628544"/>
+        <c:axId val="8861562"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="27635355"/>
+        <c:axId val="94628544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1154,12 +1162,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54158381"/>
+        <c:crossAx val="8861562"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54158381"/>
+        <c:axId val="8861562"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1196,7 +1204,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27635355"/>
+        <c:crossAx val="94628544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1337,10 +1345,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:E44"/>
+  <dimension ref="A3:F44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1619,7 +1627,11 @@
         <v>21987</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F25" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>0.05</v>
@@ -1636,6 +1648,10 @@
       <c r="E26" s="0" t="n">
         <v>990</v>
       </c>
+      <c r="F26" s="4" t="n">
+        <f aca="false">E26/(200*19.2)</f>
+        <v>0.2578125</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -1653,6 +1669,10 @@
       <c r="E27" s="0" t="n">
         <v>1054</v>
       </c>
+      <c r="F27" s="4" t="n">
+        <f aca="false">E27/(200*19.2)</f>
+        <v>0.274479166666667</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -1670,6 +1690,10 @@
       <c r="E28" s="0" t="n">
         <v>1118</v>
       </c>
+      <c r="F28" s="4" t="n">
+        <f aca="false">E28/(200*19.2)</f>
+        <v>0.291145833333333</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -1687,6 +1711,10 @@
       <c r="E29" s="0" t="n">
         <v>1181</v>
       </c>
+      <c r="F29" s="4" t="n">
+        <f aca="false">E29/(200*19.2)</f>
+        <v>0.307552083333333</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -1704,6 +1732,10 @@
       <c r="E30" s="0" t="n">
         <v>1242</v>
       </c>
+      <c r="F30" s="4" t="n">
+        <f aca="false">E30/(200*19.2)</f>
+        <v>0.3234375</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -1721,6 +1753,10 @@
       <c r="E31" s="0" t="n">
         <v>1303</v>
       </c>
+      <c r="F31" s="4" t="n">
+        <f aca="false">E31/(200*19.2)</f>
+        <v>0.339322916666667</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -1738,6 +1774,10 @@
       <c r="E32" s="0" t="n">
         <v>1363</v>
       </c>
+      <c r="F32" s="4" t="n">
+        <f aca="false">E32/(200*19.2)</f>
+        <v>0.354947916666667</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -1755,6 +1795,10 @@
       <c r="E33" s="0" t="n">
         <v>1421</v>
       </c>
+      <c r="F33" s="4" t="n">
+        <f aca="false">E33/(200*19.2)</f>
+        <v>0.370052083333333</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -1772,6 +1816,10 @@
       <c r="E34" s="0" t="n">
         <v>1478</v>
       </c>
+      <c r="F34" s="4" t="n">
+        <f aca="false">E34/(200*19.2)</f>
+        <v>0.384895833333333</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -1789,6 +1837,10 @@
       <c r="E35" s="0" t="n">
         <v>1534</v>
       </c>
+      <c r="F35" s="4" t="n">
+        <f aca="false">E35/(200*19.2)</f>
+        <v>0.399479166666667</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -1806,6 +1858,10 @@
       <c r="E36" s="0" t="n">
         <v>1589</v>
       </c>
+      <c r="F36" s="4" t="n">
+        <f aca="false">E36/(200*19.2)</f>
+        <v>0.413802083333333</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -1823,6 +1879,10 @@
       <c r="E37" s="0" t="n">
         <v>1642</v>
       </c>
+      <c r="F37" s="4" t="n">
+        <f aca="false">E37/(200*19.2)</f>
+        <v>0.427604166666667</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
@@ -1840,6 +1900,10 @@
       <c r="E38" s="0" t="n">
         <v>1693</v>
       </c>
+      <c r="F38" s="4" t="n">
+        <f aca="false">E38/(200*19.2)</f>
+        <v>0.440885416666667</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
@@ -1857,6 +1921,10 @@
       <c r="E39" s="0" t="n">
         <v>1744</v>
       </c>
+      <c r="F39" s="4" t="n">
+        <f aca="false">E39/(200*19.2)</f>
+        <v>0.454166666666667</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -1874,6 +1942,10 @@
       <c r="E40" s="0" t="n">
         <v>1792</v>
       </c>
+      <c r="F40" s="4" t="n">
+        <f aca="false">E40/(200*19.2)</f>
+        <v>0.466666666666667</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -1891,6 +1963,10 @@
       <c r="E41" s="0" t="n">
         <v>1838</v>
       </c>
+      <c r="F41" s="4" t="n">
+        <f aca="false">E41/(200*19.2)</f>
+        <v>0.478645833333333</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -1908,6 +1984,10 @@
       <c r="E42" s="0" t="n">
         <v>1883</v>
       </c>
+      <c r="F42" s="4" t="n">
+        <f aca="false">E42/(200*19.2)</f>
+        <v>0.490364583333333</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -1925,6 +2005,10 @@
       <c r="E43" s="0" t="n">
         <v>1926</v>
       </c>
+      <c r="F43" s="4" t="n">
+        <f aca="false">E43/(200*19.2)</f>
+        <v>0.5015625</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -1941,6 +2025,10 @@
       </c>
       <c r="E44" s="0" t="n">
         <v>1966</v>
+      </c>
+      <c r="F44" s="4" t="n">
+        <f aca="false">E44/(200*19.2)</f>
+        <v>0.511979166666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>